<commit_message>
Agregué el archivo de configuración
</commit_message>
<xml_diff>
--- a/busqueda.xlsx
+++ b/busqueda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nueva carpeta\PRUEBAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21902DA-9CCB-4E61-A512-6A44331BC01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16650055-26DB-4B59-88CD-4948FBB46B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{98ACAB3F-5077-42F6-95CC-4B18A0023D66}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="246">
   <si>
     <t>ITEM</t>
   </si>
@@ -751,13 +751,25 @@
   </si>
   <si>
     <t>999999990000050729391234</t>
+  </si>
+  <si>
+    <t>69790</t>
+  </si>
+  <si>
+    <t>8792</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>9522450</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -787,6 +799,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto Condensed"/>
     </font>
   </fonts>
   <fills count="5">
@@ -842,7 +860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -866,6 +884,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1202,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA0560F-908B-4C88-A2BE-C52C53E2AB78}">
   <dimension ref="A1:X846"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13.8"/>
@@ -3287,31 +3308,55 @@
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
     </row>
-    <row r="42" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
+    <row r="42" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A42" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="6">
+        <v>45579</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
+      <c r="U42" s="7"/>
+      <c r="V42" s="7"/>
+      <c r="W42" s="7"/>
+      <c r="X42" s="7"/>
     </row>
     <row r="43" spans="1:24" ht="15.75" customHeight="1">
       <c r="A43" s="3"/>
@@ -3450,7 +3495,7 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="9"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>

</xml_diff>

<commit_message>
Agrega requerimiento de actualizacion de valores en archivo final
</commit_message>
<xml_diff>
--- a/busqueda.xlsx
+++ b/busqueda.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nueva carpeta\PRUEBAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\.Programacion\.SMY\migracion-cobros-coactivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16650055-26DB-4B59-88CD-4948FBB46B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140A5AE5-866F-4645-ADD7-D935ADDE33C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{98ACAB3F-5077-42F6-95CC-4B18A0023D66}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{98ACAB3F-5077-42F6-95CC-4B18A0023D66}"/>
   </bookViews>
   <sheets>
     <sheet name="FEBRERO 2022" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="328">
   <si>
     <t>ITEM</t>
   </si>
@@ -75,9 +75,6 @@
     <t>VALOR COMPARENDO</t>
   </si>
   <si>
-    <t xml:space="preserve">VALOR EMBARGO </t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -763,6 +760,255 @@
   </si>
   <si>
     <t>9522450</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>100001</t>
+  </si>
+  <si>
+    <t>100002</t>
+  </si>
+  <si>
+    <t>100003</t>
+  </si>
+  <si>
+    <t>100004</t>
+  </si>
+  <si>
+    <t>100005</t>
+  </si>
+  <si>
+    <t>100006</t>
+  </si>
+  <si>
+    <t>100007</t>
+  </si>
+  <si>
+    <t>100008</t>
+  </si>
+  <si>
+    <t>100009</t>
+  </si>
+  <si>
+    <t>100010</t>
+  </si>
+  <si>
+    <t>100011</t>
+  </si>
+  <si>
+    <t>100012</t>
+  </si>
+  <si>
+    <t>100013</t>
+  </si>
+  <si>
+    <t>100014</t>
+  </si>
+  <si>
+    <t>100015</t>
+  </si>
+  <si>
+    <t>100016</t>
+  </si>
+  <si>
+    <t>100017</t>
+  </si>
+  <si>
+    <t>100018</t>
+  </si>
+  <si>
+    <t>100019</t>
+  </si>
+  <si>
+    <t>100020</t>
+  </si>
+  <si>
+    <t>100021</t>
+  </si>
+  <si>
+    <t>100022</t>
+  </si>
+  <si>
+    <t>100023</t>
+  </si>
+  <si>
+    <t>100024</t>
+  </si>
+  <si>
+    <t>100025</t>
+  </si>
+  <si>
+    <t>100026</t>
+  </si>
+  <si>
+    <t>100027</t>
+  </si>
+  <si>
+    <t>100028</t>
+  </si>
+  <si>
+    <t>100029</t>
+  </si>
+  <si>
+    <t>100030</t>
+  </si>
+  <si>
+    <t>100031</t>
+  </si>
+  <si>
+    <t>100032</t>
+  </si>
+  <si>
+    <t>100033</t>
+  </si>
+  <si>
+    <t>100034</t>
+  </si>
+  <si>
+    <t>100035</t>
+  </si>
+  <si>
+    <t>100036</t>
+  </si>
+  <si>
+    <t>100037</t>
+  </si>
+  <si>
+    <t>100038</t>
+  </si>
+  <si>
+    <t>100039</t>
+  </si>
+  <si>
+    <t>100040</t>
+  </si>
+  <si>
+    <t>20000001</t>
+  </si>
+  <si>
+    <t>20000002</t>
+  </si>
+  <si>
+    <t>20000003</t>
+  </si>
+  <si>
+    <t>20000004</t>
+  </si>
+  <si>
+    <t>20000005</t>
+  </si>
+  <si>
+    <t>20000006</t>
+  </si>
+  <si>
+    <t>20000007</t>
+  </si>
+  <si>
+    <t>20000008</t>
+  </si>
+  <si>
+    <t>20000009</t>
+  </si>
+  <si>
+    <t>20000010</t>
+  </si>
+  <si>
+    <t>20000011</t>
+  </si>
+  <si>
+    <t>20000012</t>
+  </si>
+  <si>
+    <t>20000013</t>
+  </si>
+  <si>
+    <t>20000014</t>
+  </si>
+  <si>
+    <t>20000015</t>
+  </si>
+  <si>
+    <t>20000016</t>
+  </si>
+  <si>
+    <t>20000017</t>
+  </si>
+  <si>
+    <t>20000018</t>
+  </si>
+  <si>
+    <t>20000019</t>
+  </si>
+  <si>
+    <t>20000020</t>
+  </si>
+  <si>
+    <t>20000021</t>
+  </si>
+  <si>
+    <t>20000022</t>
+  </si>
+  <si>
+    <t>20000023</t>
+  </si>
+  <si>
+    <t>20000024</t>
+  </si>
+  <si>
+    <t>20000025</t>
+  </si>
+  <si>
+    <t>20000026</t>
+  </si>
+  <si>
+    <t>20000027</t>
+  </si>
+  <si>
+    <t>20000028</t>
+  </si>
+  <si>
+    <t>20000029</t>
+  </si>
+  <si>
+    <t>20000030</t>
+  </si>
+  <si>
+    <t>20000031</t>
+  </si>
+  <si>
+    <t>20000032</t>
+  </si>
+  <si>
+    <t>20000033</t>
+  </si>
+  <si>
+    <t>20000034</t>
+  </si>
+  <si>
+    <t>20000035</t>
+  </si>
+  <si>
+    <t>20000036</t>
+  </si>
+  <si>
+    <t>20000037</t>
+  </si>
+  <si>
+    <t>20000038</t>
+  </si>
+  <si>
+    <t>20000039</t>
+  </si>
+  <si>
+    <t>20000040</t>
+  </si>
+  <si>
+    <t>20000041</t>
+  </si>
+  <si>
+    <t>VALOR_EMBARGO</t>
   </si>
 </sst>
 </file>
@@ -1223,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA0560F-908B-4C88-A2BE-C52C53E2AB78}">
   <dimension ref="A1:X846"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13.8"/>
@@ -1244,8 +1490,9 @@
     <col min="13" max="13" width="63.09765625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.69921875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="24" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="27.09765625" customWidth="1"/>
+    <col min="17" max="17" width="35.3984375" customWidth="1"/>
+    <col min="18" max="24" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.6">
@@ -1298,7 +1545,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>16</v>
+        <v>327</v>
       </c>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
@@ -1310,46 +1557,50 @@
     </row>
     <row r="2" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="J2" s="6">
         <v>45541</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
+      <c r="P2" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>286</v>
+      </c>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
@@ -1360,46 +1611,50 @@
     </row>
     <row r="3" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="I3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" s="6">
         <v>45542</v>
       </c>
       <c r="K3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
+      <c r="P3" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>287</v>
+      </c>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
@@ -1410,46 +1665,50 @@
     </row>
     <row r="4" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="H4" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="6">
         <v>45543</v>
       </c>
       <c r="K4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
+      <c r="P4" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>288</v>
+      </c>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
@@ -1460,46 +1719,50 @@
     </row>
     <row r="5" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="H5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" s="6">
         <v>45544</v>
       </c>
       <c r="K5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
+      <c r="P5" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>289</v>
+      </c>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
@@ -1510,46 +1773,50 @@
     </row>
     <row r="6" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J6" s="6">
         <v>45545</v>
       </c>
       <c r="K6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M6" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="P6" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
@@ -1560,46 +1827,50 @@
     </row>
     <row r="7" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="6">
         <v>45546</v>
       </c>
       <c r="K7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
+      <c r="P7" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>291</v>
+      </c>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
@@ -1610,46 +1881,50 @@
     </row>
     <row r="8" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="I8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="6">
         <v>45547</v>
       </c>
       <c r="K8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
+      <c r="P8" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>292</v>
+      </c>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
@@ -1660,46 +1935,50 @@
     </row>
     <row r="9" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="C9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" s="6">
         <v>45548</v>
       </c>
       <c r="K9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
+      <c r="P9" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>293</v>
+      </c>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
@@ -1710,46 +1989,50 @@
     </row>
     <row r="10" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="I10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J10" s="6">
         <v>45549</v>
       </c>
       <c r="K10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M10" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
+      <c r="P10" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>294</v>
+      </c>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
@@ -1760,46 +2043,50 @@
     </row>
     <row r="11" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="I11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J11" s="6">
         <v>45550</v>
       </c>
       <c r="K11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M11" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
+      <c r="P11" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>295</v>
+      </c>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
@@ -1810,46 +2097,50 @@
     </row>
     <row r="12" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="I12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J12" s="6">
         <v>45551</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
+      <c r="P12" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>296</v>
+      </c>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
@@ -1860,46 +2151,50 @@
     </row>
     <row r="13" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="I13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J13" s="6">
         <v>45552</v>
       </c>
       <c r="K13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M13" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
+      <c r="P13" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>297</v>
+      </c>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
@@ -1910,46 +2205,50 @@
     </row>
     <row r="14" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A14" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="I14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" s="6">
         <v>45553</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M14" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
+      <c r="P14" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>298</v>
+      </c>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
@@ -1960,46 +2259,50 @@
     </row>
     <row r="15" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="I15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" s="6">
         <v>45554</v>
       </c>
       <c r="K15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M15" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
+      <c r="P15" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>299</v>
+      </c>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
@@ -2010,46 +2313,50 @@
     </row>
     <row r="16" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="I16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J16" s="6">
         <v>45555</v>
       </c>
       <c r="K16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M16" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
+      <c r="P16" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>300</v>
+      </c>
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
@@ -2060,46 +2367,50 @@
     </row>
     <row r="17" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A17" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="I17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J17" s="6">
         <v>45556</v>
       </c>
       <c r="K17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M17" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
+      <c r="P17" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>301</v>
+      </c>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
@@ -2110,46 +2421,50 @@
     </row>
     <row r="18" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="C18" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J18" s="6">
         <v>45557</v>
       </c>
       <c r="K18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M18" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
+      <c r="P18" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>302</v>
+      </c>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
@@ -2160,46 +2475,50 @@
     </row>
     <row r="19" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A19" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="C19" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J19" s="6">
         <v>45558</v>
       </c>
       <c r="K19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M19" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
+      <c r="P19" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>303</v>
+      </c>
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
@@ -2210,46 +2529,50 @@
     </row>
     <row r="20" spans="1:24" s="8" customFormat="1" ht="15.6">
       <c r="A20" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="I20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J20" s="6">
         <v>45559</v>
       </c>
       <c r="K20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L20" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M20" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
+      <c r="P20" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>304</v>
+      </c>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
@@ -2260,46 +2583,50 @@
     </row>
     <row r="21" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="I21" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J21" s="6">
         <v>45560</v>
       </c>
       <c r="K21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M21" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
+      <c r="P21" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>305</v>
+      </c>
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
@@ -2310,46 +2637,50 @@
     </row>
     <row r="22" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>131</v>
-      </c>
       <c r="I22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J22" s="6">
         <v>45561</v>
       </c>
       <c r="K22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M22" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
+      <c r="P22" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>306</v>
+      </c>
       <c r="R22" s="7"/>
       <c r="S22" s="7"/>
       <c r="T22" s="7"/>
@@ -2360,46 +2691,50 @@
     </row>
     <row r="23" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="I23" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J23" s="6">
         <v>45562</v>
       </c>
       <c r="K23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M23" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
+      <c r="P23" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>307</v>
+      </c>
       <c r="R23" s="7"/>
       <c r="S23" s="7"/>
       <c r="T23" s="7"/>
@@ -2410,46 +2745,50 @@
     </row>
     <row r="24" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>143</v>
-      </c>
       <c r="I24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J24" s="6">
         <v>45563</v>
       </c>
       <c r="K24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L24" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M24" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
+      <c r="P24" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>308</v>
+      </c>
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
@@ -2460,46 +2799,50 @@
     </row>
     <row r="25" spans="1:24" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>149</v>
-      </c>
       <c r="I25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J25" s="6">
         <v>45564</v>
       </c>
       <c r="K25" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="M25" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
+      <c r="P25" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>309</v>
+      </c>
       <c r="R25" s="7"/>
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
@@ -2510,46 +2853,50 @@
     </row>
     <row r="26" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A26" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="C26" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J26" s="6">
         <v>45565</v>
       </c>
       <c r="K26" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="M26" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
+      <c r="P26" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>310</v>
+      </c>
       <c r="R26" s="7"/>
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
@@ -2560,46 +2907,50 @@
     </row>
     <row r="27" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>160</v>
-      </c>
       <c r="I27" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J27" s="6">
         <v>45566</v>
       </c>
       <c r="K27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M27" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
+      <c r="P27" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>311</v>
+      </c>
       <c r="R27" s="7"/>
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
@@ -2610,46 +2961,50 @@
     </row>
     <row r="28" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A28" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>164</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>166</v>
-      </c>
       <c r="I28" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J28" s="6">
         <v>45567</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L28" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="M28" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
+      <c r="P28" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q28" s="7" t="s">
+        <v>312</v>
+      </c>
       <c r="R28" s="7"/>
       <c r="S28" s="7"/>
       <c r="T28" s="7"/>
@@ -2660,46 +3015,50 @@
     </row>
     <row r="29" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>170</v>
-      </c>
       <c r="C29" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J29" s="6">
         <v>45568</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L29" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="M29" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="M29" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
+      <c r="P29" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="R29" s="7"/>
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
@@ -2710,46 +3069,50 @@
     </row>
     <row r="30" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="I30" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J30" s="6">
         <v>45569</v>
       </c>
       <c r="K30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M30" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
+      <c r="P30" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>314</v>
+      </c>
       <c r="R30" s="7"/>
       <c r="S30" s="7"/>
       <c r="T30" s="7"/>
@@ -2760,46 +3123,50 @@
     </row>
     <row r="31" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="C31" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>182</v>
-      </c>
       <c r="I31" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J31" s="6">
         <v>45570</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L31" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>184</v>
       </c>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
+      <c r="P31" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>315</v>
+      </c>
       <c r="R31" s="7"/>
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
@@ -2810,46 +3177,50 @@
     </row>
     <row r="32" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>189</v>
-      </c>
       <c r="I32" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J32" s="6">
         <v>45571</v>
       </c>
       <c r="K32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L32" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M32" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
+      <c r="P32" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q32" s="7" t="s">
+        <v>316</v>
+      </c>
       <c r="R32" s="7"/>
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
@@ -2860,46 +3231,50 @@
     </row>
     <row r="33" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>195</v>
-      </c>
       <c r="I33" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J33" s="6">
         <v>45572</v>
       </c>
       <c r="K33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L33" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M33" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
+      <c r="P33" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q33" s="7" t="s">
+        <v>317</v>
+      </c>
       <c r="R33" s="7"/>
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
@@ -2910,46 +3285,50 @@
     </row>
     <row r="34" spans="1:24" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="A34" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>199</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>201</v>
-      </c>
       <c r="I34" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J34" s="6">
         <v>45573</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
+      <c r="P34" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q34" s="7" t="s">
+        <v>318</v>
+      </c>
       <c r="R34" s="7"/>
       <c r="S34" s="7"/>
       <c r="T34" s="7"/>
@@ -2960,46 +3339,50 @@
     </row>
     <row r="35" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>204</v>
-      </c>
       <c r="C35" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J35" s="6">
         <v>45574</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="7"/>
+      <c r="P35" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q35" s="7" t="s">
+        <v>319</v>
+      </c>
       <c r="R35" s="7"/>
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
@@ -3010,46 +3393,50 @@
     </row>
     <row r="36" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="G36" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>211</v>
-      </c>
       <c r="I36" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J36" s="6">
         <v>45575</v>
       </c>
       <c r="K36" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="L36" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="L36" s="5" t="s">
+      <c r="M36" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>214</v>
       </c>
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
+      <c r="P36" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q36" s="7" t="s">
+        <v>320</v>
+      </c>
       <c r="R36" s="7"/>
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
@@ -3060,46 +3447,50 @@
     </row>
     <row r="37" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="C37" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J37" s="6">
         <v>45576</v>
       </c>
       <c r="K37" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="L37" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="L37" s="5" t="s">
-        <v>213</v>
-      </c>
       <c r="M37" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="7"/>
+      <c r="P37" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q37" s="7" t="s">
+        <v>321</v>
+      </c>
       <c r="R37" s="7"/>
       <c r="S37" s="7"/>
       <c r="T37" s="7"/>
@@ -3110,46 +3501,50 @@
     </row>
     <row r="38" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A38" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>220</v>
-      </c>
       <c r="C38" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J38" s="6">
         <v>45577</v>
       </c>
       <c r="K38" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="L38" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="L38" s="5" t="s">
-        <v>213</v>
-      </c>
       <c r="M38" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N38" s="7"/>
       <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
+      <c r="P38" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q38" s="7" t="s">
+        <v>322</v>
+      </c>
       <c r="R38" s="7"/>
       <c r="S38" s="7"/>
       <c r="T38" s="7"/>
@@ -3160,46 +3555,50 @@
     </row>
     <row r="39" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C39" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="G39" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>226</v>
-      </c>
       <c r="I39" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J39" s="6">
         <v>45578</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N39" s="7"/>
       <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
+      <c r="P39" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q39" s="7" t="s">
+        <v>323</v>
+      </c>
       <c r="R39" s="7"/>
       <c r="S39" s="7"/>
       <c r="T39" s="7"/>
@@ -3210,46 +3609,50 @@
     </row>
     <row r="40" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>231</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="G40" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>233</v>
-      </c>
       <c r="I40" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J40" s="6">
         <v>45579</v>
       </c>
       <c r="K40" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L40" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M40" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N40" s="7"/>
       <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
+      <c r="P40" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q40" s="7" t="s">
+        <v>324</v>
+      </c>
       <c r="R40" s="7"/>
       <c r="S40" s="7"/>
       <c r="T40" s="7"/>
@@ -3260,46 +3663,50 @@
     </row>
     <row r="41" spans="1:24" ht="15.75" customHeight="1">
       <c r="A41" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="D41" s="5" t="s">
         <v>236</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>237</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H41" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="I41" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="J41" s="6">
         <v>45580</v>
       </c>
       <c r="K41" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L41" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L41" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M41" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
+      <c r="P41" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>325</v>
+      </c>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
@@ -3310,46 +3717,50 @@
     </row>
     <row r="42" spans="1:24" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A42" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>245</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J42" s="6">
         <v>45579</v>
       </c>
       <c r="K42" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L42" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L42" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="M42" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N42" s="7"/>
       <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
+      <c r="P42" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q42" s="7" t="s">
+        <v>326</v>
+      </c>
       <c r="R42" s="7"/>
       <c r="S42" s="7"/>
       <c r="T42" s="7"/>

</xml_diff>